<commit_message>
WP Bookmarks and RemoveDuplicates added
</commit_message>
<xml_diff>
--- a/src/main/java/Bookmark/BookmarkDirectories.xlsx
+++ b/src/main/java/Bookmark/BookmarkDirectories.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitha\OneDrive\Desktop\acrobat-sign-main\sdks\PdfBox\src\main\java\Bookmark\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitha\IdeaProjects\PdfBox\src\main\java\Bookmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688CE1F8-F9DE-4F2D-9456-273AEE0E97D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5160" yWindow="3555" windowWidth="21600" windowHeight="11295" xr2:uid="{65025B94-C6C8-4E06-BE69-15070D4E9D58}"/>
+    <workbookView xWindow="5160" yWindow="3555" windowWidth="21600" windowHeight="11295"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,96 +24,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>C:\Users\mitha\OneDrive\Desktop\OE-ICP\OCR\Remaining\OCR_icp 318.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\mitha\OneDrive\Desktop\OE-ICP\OCR\Remaining\OCR_icp 319.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\mitha\OneDrive\Desktop\OE-ICP\OCR\Remaining\OCR_icp 320.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\mitha\OneDrive\Desktop\OE-ICP\OCR\Remaining\OCR_icp 321.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\mitha\OneDrive\Desktop\OE-ICP\OCR\Remaining\OCR_icp 322.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\mitha\OneDrive\Desktop\OE-ICP\OCR\Remaining\OCR_icp 323.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\mitha\OneDrive\Desktop\OE-ICP\OCR\Remaining\OCR_icp 324.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\mitha\OneDrive\Desktop\OE-ICP\OCR\Remaining\OCR_icp 325.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\mitha\OneDrive\Desktop\OE-ICP\OCR\Remaining\OCR_icp 326.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\mitha\OneDrive\Desktop\OE-ICP\OCR\Remaining\OCR_icp 327.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\mitha\OneDrive\Desktop\OE-ICP\OCR\Remaining\OCR_icp 328.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\mitha\OneDrive\Desktop\OE-ICP\OCR\Remaining\OCR_icp 329.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\mitha\OneDrive\Desktop\OE-ICP\OCR\Remaining\OCR_icp 330.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\mitha\OneDrive\Desktop\OE-ICP\OCR\Remaining\OCR_icp 331-341.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\mitha\OneDrive\Desktop\OE-ICP\OCR\Remaining\OCR_icp 342.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\mitha\OneDrive\Desktop\OE-ICP\OCR\Remaining\OCR_icp 357.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\mitha\OneDrive\Desktop\OE-ICP\OCR\Remaining\OCR_icp 358.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\mitha\OneDrive\Desktop\OE-ICP\OCR\Remaining\OCR_icp 359.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\mitha\OneDrive\Desktop\OE-ICP\OCR\Remaining\OCR_icp 360.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\mitha\OneDrive\Desktop\OE-ICP\OCR\Remaining\OCR_icp 361.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\mitha\OneDrive\Desktop\OE-ICP\OCR\Remaining\OCR_icp 362.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\mitha\OneDrive\Desktop\OE-ICP\OCR\Remaining\OCR_icp 363.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\mitha\OneDrive\Desktop\OE-ICP\OCR\Remaining\OCR_icp 364.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\mitha\OneDrive\Desktop\OE-ICP\OCR\Remaining\OCR_icp 365.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\mitha\OneDrive\Desktop\OE-ICP\OCR\Remaining\OCR_icp 366.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\mitha\OneDrive\Desktop\OE-ICP\OCR\Remaining\OCR_icp 367-385.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\mitha\OneDrive\Desktop\OE-ICP\OCR\Remaining\OCR_icp 386.pdf</t>
-  </si>
-  <si>
-    <t>C:\Users\mitha\OneDrive\Desktop\OE-ICP\OCR\Remaining\OCR_icp 387.pdf</t>
+    <t>C:\Users\martin.asenov\Desktop\PROJECTS\SEASON 4\OE-IJH\OE-IJH-H-22_Locked_24.04.2023.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -459,12 +377,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{577FB785-BB58-44DA-ACB1-F1CA44298AA7}">
-  <dimension ref="A1:A28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection sqref="A1:A28"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -476,141 +392,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>27</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
AddBookmarksAndText skip numbers added
</commit_message>
<xml_diff>
--- a/src/main/java/Bookmark/BookmarkDirectories.xlsx
+++ b/src/main/java/Bookmark/BookmarkDirectories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitha\IdeaProjects\PdfBox\src\main\java\Bookmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3564235C-30DD-40B8-80DD-11E2476C06F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3339D7A6-1F4E-4B12-8BFA-D34E9E9F4076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -381,9 +381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Add WP bookmarks adjusted
</commit_message>
<xml_diff>
--- a/src/main/java/Bookmark/BookmarkDirectories.xlsx
+++ b/src/main/java/Bookmark/BookmarkDirectories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitha\IdeaProjects\PdfBox\src\main\java\Bookmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3339D7A6-1F4E-4B12-8BFA-D34E9E9F4076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230AB715-C058-4C06-82D9-AB51E66890B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>C:\Users\mitha\Downloads\OE-ICA_6Y Check.pdf</t>
+    <t>C:\Users\mitha\OneDrive\Desktop\OE-IDU\Proper Seq\OE-IDU WP right seq.pdf</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
problems with maven are fixed
</commit_message>
<xml_diff>
--- a/src/main/java/Bookmark/BookmarkDirectories.xlsx
+++ b/src/main/java/Bookmark/BookmarkDirectories.xlsx
@@ -1,24 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitha\IdeaProjects\PdfBox\src\main\java\Bookmark\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin.asenov\IdeaProjects\PdfBox\src\main\java\Bookmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DAD455D-F738-457B-88E6-487422B535D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E531031-5A5A-46E7-844B-46654890827D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -27,7 +38,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>C:\Users\mitha\OneDrive\Desktop\E1-23-05-00013_OE-ICA_6Y CHECK\10_Customer_WP\WO8294_MPD WORKPACK_TC.pdf</t>
+    <t>C:\Users\martin.asenov\Desktop\Scanned\A7-MHH 106-1 to 106-39.pdf</t>
   </si>
 </sst>
 </file>
@@ -381,9 +392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Text field creator added
</commit_message>
<xml_diff>
--- a/src/main/java/Bookmark/BookmarkDirectories.xlsx
+++ b/src/main/java/Bookmark/BookmarkDirectories.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin.asenov\IdeaProjects\PdfBox\src\main\java\Bookmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AF73BC-8063-4430-A695-30A2F89ED8BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C278F23-59BB-4AA4-841E-89EEA31CC0AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32565" yWindow="1275" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>C:\Users\martin.asenov\Desktop\Tst\OE-IGL_Task import template.xlsx</t>
+    <t>C:\Users\martin.asenov\Desktop\BBJ\BBJ_Workpackage_In sequence.pdf_Bookmarked.pdf</t>
   </si>
 </sst>
 </file>
@@ -396,7 +396,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="77.5703125" customWidth="1"/>
+    <col min="1" max="1" width="99.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>